<commit_message>
added click to view and delete option
</commit_message>
<xml_diff>
--- a/uploads/report.xlsx
+++ b/uploads/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="91">
   <si>
     <t>AN</t>
   </si>
@@ -70,10 +70,10 @@
     <t>Net</t>
   </si>
   <si>
-    <t>Edward Chua</t>
+    <t>edrichhans</t>
   </si>
   <si>
-    <t>edrichhans</t>
+    <t>Edward Chua</t>
   </si>
   <si>
     <t>March 23, 2017</t>
@@ -665,7 +665,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S23"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -740,84 +740,120 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>451</v>
+        <v>454</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>14500</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>290</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>526.8</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="P2">
         <v>290</v>
       </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1078.2</v>
+      </c>
+      <c r="R2">
+        <v>774.93</v>
       </c>
       <c r="S2">
-        <v>1208.3333333333333</v>
+        <v>12503.27</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>452</v>
+        <v>454</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>14500</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>290</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>526.8</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="P3">
         <v>290</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1078.2</v>
+      </c>
+      <c r="R3">
+        <v>774.93</v>
       </c>
       <c r="S3">
-        <v>1208.3333333333333</v>
+        <v>12503.27</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -825,13 +861,13 @@
         <v>454</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4">
         <v>14500</v>
@@ -884,13 +920,13 @@
         <v>454</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>14500</v>
@@ -943,13 +979,13 @@
         <v>454</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>14500</v>
@@ -1002,13 +1038,13 @@
         <v>454</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E7">
         <v>14500</v>
@@ -1061,13 +1097,13 @@
         <v>454</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>14500</v>
@@ -1120,13 +1156,13 @@
         <v>454</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9">
         <v>14500</v>
@@ -1179,13 +1215,13 @@
         <v>454</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10">
         <v>14500</v>
@@ -1238,13 +1274,13 @@
         <v>454</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E11">
         <v>14500</v>
@@ -1297,13 +1333,13 @@
         <v>454</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>14500</v>
@@ -1356,13 +1392,13 @@
         <v>454</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13">
         <v>14500</v>
@@ -1415,13 +1451,13 @@
         <v>454</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <v>14500</v>
@@ -1474,13 +1510,13 @@
         <v>454</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>14500</v>
@@ -1533,34 +1569,34 @@
         <v>454</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>14500</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I16" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="J16" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="K16" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="L16">
         <v>175</v>
@@ -1584,7 +1620,7 @@
         <v>774.93</v>
       </c>
       <c r="S16">
-        <v>12503.27</v>
+        <v>11853.27</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1592,13 +1628,13 @@
         <v>454</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>14500</v>
@@ -1651,34 +1687,34 @@
         <v>454</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18">
         <v>14500</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="J18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="K18" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="L18">
         <v>175</v>
@@ -1702,7 +1738,7 @@
         <v>774.93</v>
       </c>
       <c r="S18">
-        <v>11853.27</v>
+        <v>12503.27</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1710,13 +1746,13 @@
         <v>454</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E19">
         <v>14500</v>
@@ -1769,13 +1805,13 @@
         <v>454</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20">
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20">
         <v>14500</v>
@@ -1828,13 +1864,13 @@
         <v>454</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21">
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21">
         <v>14500</v>
@@ -1887,13 +1923,13 @@
         <v>454</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22">
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E22">
         <v>14500</v>
@@ -1946,34 +1982,34 @@
         <v>454</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C23">
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E23">
         <v>14500</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="H23" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="I23" t="s">
         <v>23</v>
       </c>
       <c r="J23" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="K23" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="L23">
         <v>175</v>
@@ -1997,124 +2033,6 @@
         <v>774.93</v>
       </c>
       <c r="S23">
-        <v>12503.27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>454</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24">
-        <v>6</v>
-      </c>
-      <c r="D24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24">
-        <v>14500</v>
-      </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" t="s">
-        <v>24</v>
-      </c>
-      <c r="K24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24">
-        <v>175</v>
-      </c>
-      <c r="M24">
-        <v>290</v>
-      </c>
-      <c r="N24">
-        <v>526.8</v>
-      </c>
-      <c r="O24">
-        <v>175</v>
-      </c>
-      <c r="P24">
-        <v>290</v>
-      </c>
-      <c r="Q24">
-        <v>1078.2</v>
-      </c>
-      <c r="R24">
-        <v>774.93</v>
-      </c>
-      <c r="S24">
-        <v>12503.27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>454</v>
-      </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25">
-        <v>14500</v>
-      </c>
-      <c r="F25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" t="s">
-        <v>35</v>
-      </c>
-      <c r="K25" t="s">
-        <v>36</v>
-      </c>
-      <c r="L25">
-        <v>175</v>
-      </c>
-      <c r="M25">
-        <v>290</v>
-      </c>
-      <c r="N25">
-        <v>526.8</v>
-      </c>
-      <c r="O25">
-        <v>175</v>
-      </c>
-      <c r="P25">
-        <v>290</v>
-      </c>
-      <c r="Q25">
-        <v>1078.2</v>
-      </c>
-      <c r="R25">
-        <v>774.93</v>
-      </c>
-      <c r="S25">
         <v>12443.27</v>
       </c>
     </row>
@@ -2196,7 +2114,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -2236,7 +2154,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>53</v>
@@ -5508,7 +5426,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>55</v>
@@ -5528,7 +5446,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>69</v>
@@ -5588,7 +5506,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>77</v>
@@ -5628,7 +5546,7 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
         <v>81</v>
@@ -8815,7 +8733,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
         <v>83</v>
@@ -8835,7 +8753,7 @@
         <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
         <v>85</v>

</xml_diff>

<commit_message>
log.log and excel dl test
</commit_message>
<xml_diff>
--- a/uploads/report.xlsx
+++ b/uploads/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
   <si>
     <t>AN</t>
   </si>
@@ -162,9 +162,7 @@
   <si>
     <t>food</t>
   </si>
-  <si>
-    <t/>
-  </si>
+  <si/>
   <si>
     <t>Water Company</t>
   </si>
@@ -634,7 +632,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S3"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -764,6 +762,50 @@
       </c>
       <c r="S2">
         <v>23622.95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>602</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>3000</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>60</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>-1750</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
search and pagination in petty cash view
</commit_message>
<xml_diff>
--- a/uploads/report.xlsx
+++ b/uploads/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="104">
   <si>
     <t>AN</t>
   </si>
@@ -94,27 +94,24 @@
     <t>[100,2000]</t>
   </si>
   <si>
-    <t>April 23, 2017</t>
-  </si>
-  <si>
-    <t>["food"]</t>
-  </si>
-  <si>
-    <t>[1000]</t>
-  </si>
-  <si>
-    <t>["none"]</t>
-  </si>
-  <si>
-    <t>[""]</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
     <t>Particulars</t>
   </si>
   <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>November 10, 2016</t>
+  </si>
+  <si>
+    <t>bla bla</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
     <t>Student B</t>
   </si>
   <si>
@@ -162,7 +159,12 @@
   <si>
     <t>["food","500"]</t>
   </si>
-  <si/>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t/>
+  </si>
   <si>
     <t>Water Company</t>
   </si>
@@ -252,6 +254,78 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>dada</t>
+  </si>
+  <si>
+    <t>April 13, 2017</t>
+  </si>
+  <si>
+    <t>adw</t>
+  </si>
+  <si>
+    <t>dw1</t>
+  </si>
+  <si>
+    <t>April 12, 2017</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>March 23, 2017</t>
+  </si>
+  <si>
+    <t>3f</t>
+  </si>
+  <si>
+    <t>dar</t>
+  </si>
+  <si>
+    <t>April 15, 2017</t>
+  </si>
+  <si>
+    <t>ril</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>April 22, 2017</t>
+  </si>
+  <si>
+    <t>real na real</t>
+  </si>
+  <si>
+    <t>fab</t>
+  </si>
+  <si>
+    <t>wfkbj</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>April 19, 2017</t>
+  </si>
+  <si>
+    <t>reeltoreal</t>
+  </si>
+  <si>
+    <t>daleee</t>
+  </si>
+  <si>
+    <t>April 20, 2017</t>
+  </si>
+  <si>
+    <t>idily</t>
+  </si>
+  <si>
+    <t>jul</t>
+  </si>
+  <si>
+    <t>ef</t>
   </si>
 </sst>
 </file>
@@ -632,7 +706,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S3"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -808,124 +882,6 @@
         <v>-1750</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>602</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>3000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4">
-        <v>437.5</v>
-      </c>
-      <c r="M4">
-        <v>2000</v>
-      </c>
-      <c r="N4">
-        <v>581.3</v>
-      </c>
-      <c r="O4">
-        <v>437.5</v>
-      </c>
-      <c r="P4">
-        <v>2000</v>
-      </c>
-      <c r="Q4">
-        <v>1208.7</v>
-      </c>
-      <c r="R4">
-        <v>25083.23</v>
-      </c>
-      <c r="S4">
-        <v>70897.97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>604</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>80</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5">
-        <v>3000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5">
-        <v>312.5</v>
-      </c>
-      <c r="M5">
-        <v>500</v>
-      </c>
-      <c r="N5">
-        <v>581.3</v>
-      </c>
-      <c r="O5">
-        <v>312.5</v>
-      </c>
-      <c r="P5">
-        <v>500</v>
-      </c>
-      <c r="Q5">
-        <v>1208.7</v>
-      </c>
-      <c r="R5">
-        <v>2083.25</v>
-      </c>
-      <c r="S5">
-        <v>21522.95</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -933,173 +889,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
-  <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>296</v>
-      </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>297</v>
-      </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8">
-        <v>500</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -1123,10 +912,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -1134,19 +923,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1154,33 +943,36 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
+        <v>34</v>
+      </c>
+      <c r="F3">
+        <v>30000</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1188,19 +980,19 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>58</v>
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1211,116 +1003,101 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F6" t="s">
-        <v>61</v>
+        <v>44</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F7" t="s">
-        <v>63</v>
+        <v>47</v>
+      </c>
+      <c r="F7">
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
+        <v>293</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" t="s">
-        <v>66</v>
+        <v>48</v>
+      </c>
+      <c r="F8">
+        <v>500</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
+        <v>295</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" t="s">
-        <v>68</v>
+        <v>47</v>
+      </c>
+      <c r="F9">
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>39</v>
+        <v>296</v>
       </c>
       <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
-        <v>69</v>
-      </c>
       <c r="E10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
+        <v>47</v>
+      </c>
+      <c r="F10">
+        <v>500</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
+        <v>297</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" t="s">
-        <v>72</v>
+        <v>47</v>
+      </c>
+      <c r="F11">
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -1329,9 +1106,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F13"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -1353,10 +1130,274 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -1416,6 +1457,194 @@
       </c>
       <c r="F5">
         <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>298</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>299</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>300</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>301</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>302</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>303</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>304</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>305</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>306</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed a few things from user acceptance
</commit_message>
<xml_diff>
--- a/uploads/report.xlsx
+++ b/uploads/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="104">
   <si>
     <t>AN</t>
   </si>
@@ -22,6 +22,9 @@
     <t>Issued By</t>
   </si>
   <si>
+    <t>Date Issued</t>
+  </si>
+  <si>
     <t>Employee ID</t>
   </si>
   <si>
@@ -70,9 +73,15 @@
     <t>Net</t>
   </si>
   <si>
+    <t>04-2017</t>
+  </si>
+  <si>
     <t>edrichhans</t>
   </si>
   <si>
+    <t>Wed Apr 05 2017 14:06:55 GMT+0800 (PHT)</t>
+  </si>
+  <si>
     <t>Adrian Sing</t>
   </si>
   <si>
@@ -82,31 +91,50 @@
     <t>April 30, 2017</t>
   </si>
   <si>
-    <t>["None"]</t>
-  </si>
-  <si>
-    <t>[0]</t>
-  </si>
-  <si>
-    <t>["Food","Place"]</t>
-  </si>
-  <si>
-    <t>[100,2000]</t>
-  </si>
-  <si>
-    <t>April 23, 2017</t>
-  </si>
-  <si>
-    <t>["food"]</t>
-  </si>
-  <si>
-    <t>[1000]</t>
-  </si>
-  <si>
-    <t>["none"]</t>
-  </si>
-  <si>
-    <t>[""]</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Place</t>
+  </si>
+  <si>
+    <t>Thu Apr 20 2017 16:43:30 GMT+0800 (PHT)</t>
+  </si>
+  <si>
+    <t>January 1, 2017</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>ni</t>
+  </si>
+  <si>
+    <t>Fri Apr 21 2017 08:07:31 GMT+0800 (PHT)</t>
+  </si>
+  <si/>
+  <si>
+    <t>Tue Apr 25 2017 09:45:52 GMT+0800 (PHT)</t>
+  </si>
+  <si>
+    <t>February 1, 2017</t>
+  </si>
+  <si>
+    <t>February 28, 2017</t>
+  </si>
+  <si>
+    <t>Marami</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Subtotal:</t>
+  </si>
+  <si>
+    <t>Total:</t>
   </si>
   <si>
     <t>Date</t>
@@ -115,6 +143,9 @@
     <t>Particulars</t>
   </si>
   <si>
+    <t>10-2016</t>
+  </si>
+  <si>
     <t>Student B</t>
   </si>
   <si>
@@ -124,6 +155,9 @@
     <t>Tuition payment</t>
   </si>
   <si>
+    <t>12-2016</t>
+  </si>
+  <si>
     <t>af</t>
   </si>
   <si>
@@ -145,13 +179,16 @@
     <t>aaa</t>
   </si>
   <si>
+    <t>02-2017</t>
+  </si>
+  <si>
     <t>qwdfsgs</t>
   </si>
   <si>
     <t>February 9, 2017</t>
   </si>
   <si>
-    <t>Food</t>
+    <t>03-2017</t>
   </si>
   <si>
     <t>Edrich Chua</t>
@@ -162,7 +199,21 @@
   <si>
     <t>["food","500"]</t>
   </si>
-  <si/>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>April 21, 2017</t>
+  </si>
+  <si>
+    <t>Tuition</t>
+  </si>
+  <si>
+    <t>aN-NaN</t>
+  </si>
+  <si>
+    <t>11-2016</t>
+  </si>
   <si>
     <t>Water Company</t>
   </si>
@@ -233,6 +284,15 @@
     <t>100</t>
   </si>
   <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>petty</t>
   </si>
   <si>
@@ -252,6 +312,18 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Goodwill</t>
+  </si>
+  <si>
+    <t>Books</t>
+  </si>
+  <si>
+    <t>Edrich</t>
+  </si>
+  <si>
+    <t>April 24, 2017</t>
   </si>
 </sst>
 </file>
@@ -632,21 +704,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:T9"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="15" customWidth="1"/>
-    <col min="11" max="19" width="10" customWidth="1"/>
+    <col min="2" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="20" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,10 +750,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>11</v>
@@ -704,226 +776,285 @@
       <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>597</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
         <v>80</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3">
         <v>3000</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>312.5</v>
+      </c>
+      <c r="N3">
+        <v>500</v>
+      </c>
+      <c r="O3">
+        <v>581.3</v>
+      </c>
+      <c r="P3">
+        <v>312.5</v>
+      </c>
+      <c r="Q3">
+        <v>500</v>
+      </c>
+      <c r="R3">
+        <v>1208.7</v>
+      </c>
+      <c r="S3">
+        <v>2083.25</v>
+      </c>
+      <c r="T3">
+        <v>23622.95</v>
+      </c>
+    </row>
+    <row r="4" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>623</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="I2" t="s">
+      <c r="F5">
+        <v>3000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5">
+        <v>1000</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <v>60</v>
+      </c>
+      <c r="O5">
+        <v>109</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="Q5">
+        <v>60</v>
+      </c>
+      <c r="R5">
+        <v>231</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>3731</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>624</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>92</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6">
+        <v>3000</v>
+      </c>
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2">
-        <v>312.5</v>
-      </c>
-      <c r="M2">
-        <v>500</v>
-      </c>
-      <c r="N2">
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6">
+        <v>1000</v>
+      </c>
+      <c r="M6">
+        <v>187.5</v>
+      </c>
+      <c r="N6">
+        <v>300</v>
+      </c>
+      <c r="O6">
+        <v>545</v>
+      </c>
+      <c r="P6">
+        <v>187.5</v>
+      </c>
+      <c r="Q6">
+        <v>300</v>
+      </c>
+      <c r="R6">
+        <v>1135</v>
+      </c>
+      <c r="S6">
+        <v>874.93</v>
+      </c>
+      <c r="T6">
+        <v>14092.57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>629</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>3000</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>437.5</v>
+      </c>
+      <c r="N7">
+        <v>4000.02</v>
+      </c>
+      <c r="O7">
         <v>581.3</v>
       </c>
-      <c r="O2">
-        <v>312.5</v>
-      </c>
-      <c r="P2">
-        <v>500</v>
-      </c>
-      <c r="Q2">
+      <c r="P7">
+        <v>437.5</v>
+      </c>
+      <c r="Q7">
+        <v>4000.02</v>
+      </c>
+      <c r="R7">
         <v>1208.7</v>
       </c>
-      <c r="R2">
-        <v>2083.25</v>
-      </c>
-      <c r="S2">
-        <v>23622.95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>602</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3">
-        <v>3000</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>60</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>-1750</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>602</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>3000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4">
-        <v>437.5</v>
-      </c>
-      <c r="M4">
-        <v>2000</v>
-      </c>
-      <c r="N4">
-        <v>581.3</v>
-      </c>
-      <c r="O4">
-        <v>437.5</v>
-      </c>
-      <c r="P4">
-        <v>2000</v>
-      </c>
-      <c r="Q4">
-        <v>1208.7</v>
-      </c>
-      <c r="R4">
-        <v>25083.23</v>
-      </c>
-      <c r="S4">
-        <v>70897.97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>604</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>80</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5">
-        <v>3000</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5">
-        <v>312.5</v>
-      </c>
-      <c r="M5">
-        <v>500</v>
-      </c>
-      <c r="N5">
-        <v>581.3</v>
-      </c>
-      <c r="O5">
-        <v>312.5</v>
-      </c>
-      <c r="P5">
-        <v>500</v>
-      </c>
-      <c r="Q5">
-        <v>1208.7</v>
-      </c>
-      <c r="R5">
-        <v>2083.25</v>
-      </c>
-      <c r="S5">
-        <v>21522.95</v>
+      <c r="S7">
+        <v>57750.43</v>
+      </c>
+      <c r="T7">
+        <v>137131.75000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T8">
+        <v>178578.27000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R9" t="s">
+        <v>40</v>
+      </c>
+      <c r="T9">
+        <v>178578.27000000002</v>
       </c>
     </row>
   </sheetData>
@@ -934,7 +1065,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F20"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -953,144 +1084,237 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2">
-        <v>30000</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="F3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="4" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
       <c r="F4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>8</v>
-      </c>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5">
-        <v>10</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>9</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>296</v>
       </c>
-      <c r="C7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7">
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>297</v>
       </c>
-      <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8">
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15">
         <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>305</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20">
+        <v>41622</v>
       </c>
     </row>
   </sheetData>
@@ -1101,7 +1325,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F21"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -1120,207 +1344,287 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>7</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F4">
+        <v>NaN</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="F8" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" t="s">
         <v>69</v>
       </c>
-      <c r="E10" t="s">
-        <v>60</v>
-      </c>
       <c r="F10" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14">
+        <v>265759</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
         <v>72</v>
+      </c>
+      <c r="F16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>302</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>
@@ -1331,7 +1635,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H16"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -1339,10 +1643,11 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="6" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1350,72 +1655,190 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
         <v>9</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2">
-        <v>1000</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="F3">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="F4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5">
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8">
         <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>305</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>313</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" t="s">
+        <v>97</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16">
+        <v>40000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed excel formatting, no download yet
</commit_message>
<xml_diff>
--- a/uploads/report.xlsx
+++ b/uploads/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="73">
   <si>
     <t>AN</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Date Issued</t>
   </si>
   <si>
-    <t>Employee ID</t>
+    <t>eID</t>
   </si>
   <si>
     <t>Name</t>
@@ -73,13 +73,13 @@
     <t>Net</t>
   </si>
   <si>
-    <t>04-2017</t>
+    <t>05-2017</t>
   </si>
   <si>
     <t>edrichhans</t>
   </si>
   <si>
-    <t>Wed Apr 05 2017 14:06:55 GMT+0800 (PHT)</t>
+    <t>May 3, 2017</t>
   </si>
   <si>
     <t>Adrian Sing</t>
@@ -97,30 +97,18 @@
     <t>Food</t>
   </si>
   <si>
+    <t>ello</t>
+  </si>
+  <si>
     <t>Place</t>
   </si>
   <si>
-    <t>Wed Apr 05 2017 20:12:08 GMT+0800 (PHT)</t>
-  </si>
-  <si>
-    <t>05-2017</t>
-  </si>
-  <si>
-    <t>Mon May 01 2017 17:05:22 GMT+0800 (PHT)</t>
-  </si>
-  <si>
     <t>May 1, 2017</t>
   </si>
   <si>
     <t>May 31, 2017</t>
   </si>
   <si>
-    <t>Mon May 01 2017 18:05:59 GMT+0800 (PHT)</t>
-  </si>
-  <si>
-    <t>Mon May 01 2017 18:08:42 GMT+0800 (PHT)</t>
-  </si>
-  <si>
     <t>Subtotal:</t>
   </si>
   <si>
@@ -172,10 +160,6 @@
     <t>food</t>
   </si>
   <si>
-    <t>aN-NaN</t>
-  </si>
-  <si/>
-  <si>
     <t>11-2016</t>
   </si>
   <si>
@@ -188,69 +172,42 @@
     <t>Utilities</t>
   </si>
   <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>Companyyyyyy</t>
   </si>
   <si>
     <t>Rental</t>
   </si>
   <si>
-    <t>100000</t>
-  </si>
-  <si>
     <t>November 11, 2016</t>
   </si>
   <si>
-    <t>23000</t>
-  </si>
-  <si>
     <t>eeeeeee</t>
   </si>
   <si>
     <t>Gov't Payables</t>
   </si>
   <si>
-    <t>1515</t>
-  </si>
-  <si>
     <t>checkvoicer</t>
   </si>
   <si>
-    <t>7777</t>
-  </si>
-  <si>
     <t>checkckckckc</t>
   </si>
   <si>
     <t>November 1, 2016</t>
   </si>
   <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>adfasdfasdfasdf</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>November 30, 2016</t>
   </si>
   <si>
-    <t>123456</t>
-  </si>
-  <si>
     <t>lla</t>
   </si>
   <si>
     <t>December 6, 2016</t>
   </si>
   <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -269,28 +226,22 @@
     <t>March 13, 2017</t>
   </si>
   <si>
-    <t>thing,</t>
-  </si>
-  <si>
-    <t>thing2</t>
-  </si>
-  <si>
-    <t>thing3</t>
-  </si>
-  <si>
-    <t>Petty cash</t>
-  </si>
-  <si>
-    <t>Lol</t>
-  </si>
-  <si>
-    <t>No</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.00;[Red]-#,##0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <color theme="1"/>
@@ -311,7 +262,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -319,13 +270,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="double"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,86 +631,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T12"/>
+  <dimension ref="A1:T7"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
     <col min="7" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="10" customWidth="1"/>
+    <col min="10" max="10" width="10" style="1" customWidth="1"/>
     <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="20" width="10" customWidth="1"/>
+    <col min="12" max="20" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>19</v>
       </c>
+      <c r="F2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -762,7 +737,7 @@
       <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>3000</v>
       </c>
       <c r="G3" t="s">
@@ -774,38 +749,38 @@
       <c r="I3" t="s">
         <v>25</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="1">
         <v>0</v>
       </c>
       <c r="K3" t="s">
         <v>26</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="1">
         <v>100</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>312.5</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>500</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <v>581.3</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="1">
         <v>312.5</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="1">
         <v>500</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="1">
         <v>1208.7</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="1">
         <v>2083.25</v>
       </c>
-      <c r="T3">
-        <v>23622.95</v>
+      <c r="T3" s="1">
+        <v>22622.95</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -814,23 +789,29 @@
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
-      <c r="F4"/>
+      <c r="F4" s="1"/>
       <c r="G4"/>
       <c r="H4"/>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1000</v>
+      </c>
       <c r="K4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4">
+        <v>28</v>
+      </c>
+      <c r="L4" s="1">
         <v>2000</v>
       </c>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-      <c r="P4"/>
-      <c r="Q4"/>
-      <c r="R4"/>
-      <c r="S4"/>
-      <c r="T4"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -840,7 +821,7 @@
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>11</v>
@@ -848,213 +829,74 @@
       <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>3000</v>
       </c>
-      <c r="M5">
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="1">
         <v>0</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <v>0</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
         <v>0</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="1">
         <v>0</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="1">
         <v>60</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="1">
         <v>0</v>
       </c>
-      <c r="T5">
-        <v>1750</v>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-      <c r="T6"/>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>603</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8">
-        <v>3000</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H8" t="s">
+      <c r="S6" s="5"/>
+      <c r="T6" s="5">
+        <v>24122.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>2000</v>
-      </c>
-      <c r="R8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>604</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9">
-        <v>3000</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>2000</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>605</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10">
-        <v>3000</v>
-      </c>
-      <c r="G10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>2000</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="11" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R11" t="s">
-        <v>35</v>
-      </c>
-      <c r="T11">
-        <v>150000</v>
-      </c>
-    </row>
-    <row r="12" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R12" t="s">
-        <v>36</v>
-      </c>
-      <c r="T12">
-        <v>175372.95</v>
+      <c r="T7" s="1">
+        <v>24122.95</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="16">
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
@@ -1071,22 +913,6 @@
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="T3:T4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="R5:R6"/>
-    <mergeCell ref="S5:S6"/>
-    <mergeCell ref="T5:T6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
@@ -1103,32 +929,32 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1136,32 +962,36 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,29 +1002,33 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1202,15 +1036,15 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9">
+        <v>46</v>
+      </c>
+      <c r="F9" s="1">
         <v>500</v>
       </c>
     </row>
@@ -1219,15 +1053,15 @@
         <v>293</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10">
+        <v>47</v>
+      </c>
+      <c r="F10" s="1">
         <v>500</v>
       </c>
     </row>
@@ -1236,15 +1070,15 @@
         <v>295</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1">
         <v>500</v>
       </c>
     </row>
@@ -1253,15 +1087,15 @@
         <v>296</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12">
+        <v>46</v>
+      </c>
+      <c r="F12" s="1">
         <v>500</v>
       </c>
     </row>
@@ -1270,31 +1104,35 @@
         <v>297</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13">
+        <v>46</v>
+      </c>
+      <c r="F13" s="1">
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="5">
         <v>2500</v>
       </c>
     </row>
     <row r="15" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15">
+        <v>32</v>
+      </c>
+      <c r="F15" s="1">
         <v>2522</v>
       </c>
     </row>
@@ -1306,7 +1144,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F19"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -1314,311 +1152,293 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="D3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4">
-        <v>NaN</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>7</v>
+      </c>
       <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
+      </c>
+      <c r="E5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="1">
+        <v>23000</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>55</v>
       </c>
       <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
         <v>56</v>
       </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" t="s">
-        <v>58</v>
+      <c r="F6" s="1">
+        <v>1515</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" t="s">
-        <v>61</v>
+        <v>51</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7777</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" t="s">
-        <v>63</v>
+        <v>53</v>
+      </c>
+      <c r="F8" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
         <v>56</v>
       </c>
-      <c r="E9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" t="s">
-        <v>66</v>
+      <c r="F9" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" t="s">
         <v>56</v>
       </c>
-      <c r="E10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" t="s">
-        <v>68</v>
+      <c r="F10" s="1">
+        <v>123456</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" t="s">
-        <v>60</v>
-      </c>
-      <c r="F11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="5">
+        <v>265759</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14">
-        <v>265759</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F13" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F16" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>45</v>
+      </c>
       <c r="E17" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s">
-        <v>49</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F17" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" t="s">
-        <v>50</v>
-      </c>
-      <c r="F20">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22">
+        <v>32</v>
+      </c>
+      <c r="F19" s="1">
         <v>1000</v>
       </c>
     </row>
@@ -1630,7 +1450,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H10"/>
   <sheetFormatPr defaultRowHeight="20" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
@@ -1638,42 +1458,42 @@
     <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="6" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>80</v>
+      <c r="G1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1681,35 +1501,44 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3">
+        <v>67</v>
+      </c>
+      <c r="F3" s="1">
         <v>1000</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>69</v>
       </c>
@@ -1717,104 +1546,72 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6">
+        <v>70</v>
+      </c>
+      <c r="F6" s="1">
         <v>100</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F7">
+        <v>71</v>
+      </c>
+      <c r="F7" s="1">
         <v>200</v>
       </c>
       <c r="G7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8">
+        <v>72</v>
+      </c>
+      <c r="F8" s="1">
         <v>300</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>298</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="H8" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11">
-        <v>1000</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F12">
-        <v>200</v>
-      </c>
-      <c r="G12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14">
-        <v>1500</v>
+      <c r="H9" s="5">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="10" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="1">
+        <v>4400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>